<commit_message>
Adds basic t-test table and updates styling
</commit_message>
<xml_diff>
--- a/SMStatsResults.xlsx
+++ b/SMStatsResults.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="37140" yWindow="2120" windowWidth="29720" windowHeight="17560" xr2:uid="{74447161-86B1-0742-A968-A7F9F686B80F}"/>
+    <workbookView xWindow="1340" yWindow="1040" windowWidth="29440" windowHeight="17740" activeTab="1" xr2:uid="{74447161-86B1-0742-A968-A7F9F686B80F}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Results" sheetId="1" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>All Santa Monica</t>
   </si>
@@ -72,18 +72,6 @@
     <t>Larceny</t>
   </si>
   <si>
-    <t>0.1038251</t>
-  </si>
-  <si>
-    <t>0.5027322</t>
-  </si>
-  <si>
-    <t>-1.20765</t>
-  </si>
-  <si>
-    <t>-1.103825</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -112,6 +100,54 @@
   </si>
   <si>
     <t>Delete 0.5-1 mile</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Within Half Mile</t>
+  </si>
+  <si>
+    <t>All Except Half Mile</t>
+  </si>
+  <si>
+    <t>*p&lt;0.1; **p&lt;0.05; ***p&lt;0.01</t>
+  </si>
+  <si>
+    <t>1.10***</t>
+  </si>
+  <si>
+    <t>0.13</t>
+  </si>
+  <si>
+    <t>0.99*</t>
+  </si>
+  <si>
+    <t>1.46***</t>
+  </si>
+  <si>
+    <t>1.21***</t>
+  </si>
+  <si>
+    <t>0.18**</t>
+  </si>
+  <si>
+    <t>1.03***</t>
+  </si>
+  <si>
+    <t>0.99***</t>
+  </si>
+  <si>
+    <t>-0.10</t>
+  </si>
+  <si>
+    <t>0.59***</t>
+  </si>
+  <si>
+    <t>0.48**</t>
+  </si>
+  <si>
+    <t>Difference in Means (Daily)</t>
   </si>
 </sst>
 </file>
@@ -120,8 +156,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -167,7 +203,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -192,16 +228,162 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="53">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -289,6 +471,216 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -394,16 +786,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{54596D3B-5767-C94A-902A-48656B317053}" name="Table1" displayName="Table1" ref="B1:I22" totalsRowShown="0" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{54596D3B-5767-C94A-902A-48656B317053}" name="Table1" displayName="Table1" ref="B1:I22" totalsRowShown="0" headerRowDxfId="52">
   <autoFilter ref="B1:I22" xr:uid="{02F9A604-82D6-9C40-A8F1-857EC5C6BB0A}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{97E23EBE-243B-5545-A2E0-87E7837BC120}" name="Column1" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{5643EECD-6EDF-5344-9BEF-4886FA1B78BF}" name="Column2" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{A91401C0-B871-3540-8903-CECD1E119065}" name="Column3" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{3AF727AF-BEC3-4448-9CBE-7487706B3624}" name="Column4" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{F743AF2C-C3AB-D04C-BF8D-11A6275DD5D0}" name="Column5" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{4B2976DA-405F-3040-B7FC-797E4E8C8464}" name="Column6" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{0DBEBA94-EF67-AB48-8513-60E94ED70521}" name="Column8" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{97E23EBE-243B-5545-A2E0-87E7837BC120}" name="Column1" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{5643EECD-6EDF-5344-9BEF-4886FA1B78BF}" name="Column2" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{A91401C0-B871-3540-8903-CECD1E119065}" name="Column3" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{3AF727AF-BEC3-4448-9CBE-7487706B3624}" name="Column4" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{F743AF2C-C3AB-D04C-BF8D-11A6275DD5D0}" name="Column5" dataDxfId="47"/>
+    <tableColumn id="6" xr3:uid="{4B2976DA-405F-3040-B7FC-797E4E8C8464}" name="Column6" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{0DBEBA94-EF67-AB48-8513-60E94ED70521}" name="Column8" dataDxfId="45"/>
     <tableColumn id="9" xr3:uid="{E4670CFB-A552-B54B-B5ED-83D93204996E}" name="Column9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -709,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FEFA464-7F8F-B64B-8875-2F96CA1A8EC6}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -726,28 +1118,28 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -773,7 +1165,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>4</v>
@@ -818,8 +1210,8 @@
       <c r="C7" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>18</v>
+      <c r="D7" s="11">
+        <v>-1.1038250000000001</v>
       </c>
       <c r="E7" s="8">
         <v>-1.9103275</v>
@@ -827,10 +1219,10 @@
       <c r="F7" s="8">
         <v>-0.2973228</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <v>-2.6913999999999998</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <v>7.4419999999999998E-3</v>
       </c>
     </row>
@@ -839,8 +1231,8 @@
       <c r="C8" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>17</v>
+      <c r="D8" s="11">
+        <v>-1.2076499999999999</v>
       </c>
       <c r="E8" s="8">
         <v>-1.7177895000000001</v>
@@ -848,23 +1240,23 @@
       <c r="F8" s="8">
         <v>-0.69751110000000005</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <v>-4.6553000000000004</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <v>4.5360000000000003E-6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>16</v>
+      <c r="D9" s="11">
+        <v>0.50273219999999996</v>
       </c>
       <c r="E9" s="8">
         <v>5.1960609999999997E-2</v>
@@ -872,10 +1264,10 @@
       <c r="F9" s="8">
         <v>0.95350387000000003</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>2.1932</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>2.8930000000000001E-2</v>
       </c>
     </row>
@@ -884,8 +1276,8 @@
       <c r="C10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>15</v>
+      <c r="D10" s="11">
+        <v>0.1038251</v>
       </c>
       <c r="E10" s="8">
         <v>-0.528443</v>
@@ -893,10 +1285,10 @@
       <c r="F10" s="8">
         <v>0.7360932</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <v>0.32291999999999998</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <v>0.74690000000000001</v>
       </c>
     </row>
@@ -907,7 +1299,7 @@
       <c r="C11" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="11">
         <v>-0.1311475</v>
       </c>
       <c r="E11" s="8">
@@ -916,10 +1308,10 @@
       <c r="F11" s="8">
         <v>0.14622080000000001</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>-0.92981000000000003</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="10">
         <v>0.35310000000000002</v>
       </c>
     </row>
@@ -928,7 +1320,7 @@
       <c r="C12" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="11">
         <v>-0.1830601</v>
       </c>
       <c r="E12" s="8">
@@ -937,10 +1329,10 @@
       <c r="F12" s="8">
         <v>-1.491202E-2</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="9">
         <v>-2.1408999999999998</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="10">
         <v>3.295E-2</v>
       </c>
     </row>
@@ -949,7 +1341,7 @@
       <c r="C13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="11">
         <v>7.3770489999999994E-2</v>
       </c>
       <c r="E13" s="8">
@@ -958,10 +1350,10 @@
       <c r="F13" s="8">
         <v>0.23364747</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="9">
         <v>0.90737999999999996</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="10">
         <v>0.36480000000000001</v>
       </c>
     </row>
@@ -970,7 +1362,7 @@
       <c r="C14" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="11">
         <v>-0.5874317</v>
       </c>
       <c r="E14" s="8">
@@ -979,10 +1371,10 @@
       <c r="F14" s="8">
         <v>-0.39791939999999998</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="9">
         <v>-6.0955000000000004</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="10">
         <v>2.775E-9</v>
       </c>
     </row>
@@ -993,7 +1385,7 @@
       <c r="C15" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="11">
         <v>-0.99180330000000005</v>
       </c>
       <c r="E15" s="8">
@@ -1002,10 +1394,10 @@
       <c r="F15" s="8">
         <v>-0.24077979999999999</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="9">
         <v>-2.5969000000000002</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="10">
         <v>9.7859999999999996E-3</v>
       </c>
     </row>
@@ -1014,7 +1406,7 @@
       <c r="C16" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="11">
         <v>-1.0273220000000001</v>
       </c>
       <c r="E16" s="8">
@@ -1023,10 +1415,10 @@
       <c r="F16" s="8">
         <v>-0.54821520000000001</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="9">
         <v>-4.2165999999999997</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="10">
         <v>3.1309999999999997E-5</v>
       </c>
     </row>
@@ -1035,7 +1427,7 @@
       <c r="C17" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="11">
         <v>0.43442619999999998</v>
       </c>
       <c r="E17" s="8">
@@ -1044,10 +1436,10 @@
       <c r="F17" s="8">
         <v>0.85124657000000004</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="9">
         <v>2.0495000000000001</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="10">
         <v>4.1119999999999997E-2</v>
       </c>
     </row>
@@ -1056,7 +1448,7 @@
       <c r="C18" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="11">
         <v>0.1038251</v>
       </c>
       <c r="E18" s="8">
@@ -1065,10 +1457,10 @@
       <c r="F18" s="8">
         <v>0.7360932</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="9">
         <v>0.32291999999999998</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="10">
         <v>0.74690000000000001</v>
       </c>
     </row>
@@ -1079,7 +1471,7 @@
       <c r="C19" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="11">
         <v>-1.4644809999999999</v>
       </c>
       <c r="E19" s="8">
@@ -1088,10 +1480,10 @@
       <c r="F19" s="8">
         <v>-1.000683</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="9">
         <v>-6.2092999999999998</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="10">
         <v>1.448E-9</v>
       </c>
     </row>
@@ -1100,7 +1492,7 @@
       <c r="C20" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="11">
         <v>-0.98907100000000003</v>
       </c>
       <c r="E20" s="8">
@@ -1110,10 +1502,10 @@
         <f>-0.6884517</f>
         <v>-0.6884517</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="9">
         <v>-6.47</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="10">
         <v>3.1570000000000001E-10</v>
       </c>
     </row>
@@ -1122,7 +1514,7 @@
       <c r="C21" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="11">
         <v>7.9234970000000002E-2</v>
       </c>
       <c r="E21" s="8">
@@ -1131,10 +1523,10 @@
       <c r="F21" s="8">
         <v>-0.32264080000000001</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="9">
         <v>0.64014000000000004</v>
       </c>
-      <c r="H21" s="11">
+      <c r="H21" s="10">
         <v>0.52249999999999996</v>
       </c>
     </row>
@@ -1143,7 +1535,7 @@
       <c r="C22" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="11">
         <v>-0.47540979999999999</v>
       </c>
       <c r="E22" s="8">
@@ -1152,35 +1544,26 @@
       <c r="F22" s="8">
         <v>-0.13927129999999999</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="9">
         <v>-2.7812999999999999</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H22" s="10">
         <v>5.6959999999999997E-3</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H7:H22">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="5" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D22">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="D7:D22" numberStoredAsText="1"/>
-  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -1189,12 +1572,114 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A14E29-F343-AA4D-9152-A6515E9E84ED}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="152" zoomScaleNormal="152" workbookViewId="0">
+      <selection sqref="A1:E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="14"/>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="14"/>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="14"/>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C8" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A3:A6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E5 E3 C4" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>